<commit_message>
little translation to bg, added more subfolders
</commit_message>
<xml_diff>
--- a/assets/DBT_s_imeili.xlsx
+++ b/assets/DBT_s_imeili.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gnikolova\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kaloyan.Valchev\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{967E2DCE-8464-451C-A6F7-837E545FFA84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,21 +21,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="317">
   <si>
     <t>DBT Sofia-Vazrazhdane</t>
   </si>
@@ -670,12 +662,327 @@
   </si>
   <si>
     <t>DBT-812@az.government.bg</t>
+  </si>
+  <si>
+    <t>ДБТ София-Възраждане</t>
+  </si>
+  <si>
+    <t>ДБТ София-Люлин</t>
+  </si>
+  <si>
+    <t>ДБТ София-Сердика</t>
+  </si>
+  <si>
+    <t>ДБТ София-Изток</t>
+  </si>
+  <si>
+    <t>ДБТ Благоевград</t>
+  </si>
+  <si>
+    <t>ДБТ Ботевград</t>
+  </si>
+  <si>
+    <t>ДБТ Гоце Делчев</t>
+  </si>
+  <si>
+    <t>ДБТ Ихтиман</t>
+  </si>
+  <si>
+    <t>ДБТ Кюстендил</t>
+  </si>
+  <si>
+    <t>ДБТ Перник</t>
+  </si>
+  <si>
+    <t>ДБТ Петрич</t>
+  </si>
+  <si>
+    <t>ДБТ Разлог</t>
+  </si>
+  <si>
+    <t>ДБТ Самоков</t>
+  </si>
+  <si>
+    <t>ДБТ Сандански</t>
+  </si>
+  <si>
+    <t>ДБТ Своге</t>
+  </si>
+  <si>
+    <t>ДБТ Сливница</t>
+  </si>
+  <si>
+    <t>ДБТ Пирдоп</t>
+  </si>
+  <si>
+    <t>ДБТ Дупница</t>
+  </si>
+  <si>
+    <t>ДБТ Ардино</t>
+  </si>
+  <si>
+    <t>ДБТ Димитровград</t>
+  </si>
+  <si>
+    <t>ДБТ Казанлък</t>
+  </si>
+  <si>
+    <t>ДБТ Кирково</t>
+  </si>
+  <si>
+    <t>ДБТ Крумовград</t>
+  </si>
+  <si>
+    <t>ДБТ Кърджали</t>
+  </si>
+  <si>
+    <t>ДБТ Момчилград</t>
+  </si>
+  <si>
+    <t>ДБТ Раднево</t>
+  </si>
+  <si>
+    <t>ДБТ Свиленград</t>
+  </si>
+  <si>
+    <t>ДБТ Стара Загора</t>
+  </si>
+  <si>
+    <t>ДБТ Харманли</t>
+  </si>
+  <si>
+    <t>ДБТ Хасково</t>
+  </si>
+  <si>
+    <t>ДБТ Чирпан</t>
+  </si>
+  <si>
+    <t>ДБТ Айтос</t>
+  </si>
+  <si>
+    <t>ДБТ Бургас</t>
+  </si>
+  <si>
+    <t>ДБТ Елхово</t>
+  </si>
+  <si>
+    <t>ДБТ Карнобат</t>
+  </si>
+  <si>
+    <t>ДБТ Поморие</t>
+  </si>
+  <si>
+    <t>ДБТ Нова Загора</t>
+  </si>
+  <si>
+    <t>ДБТ Сливен</t>
+  </si>
+  <si>
+    <t>ДБТ Ямбол</t>
+  </si>
+  <si>
+    <t>ДБТ Котел</t>
+  </si>
+  <si>
+    <t>ДБТ Руен</t>
+  </si>
+  <si>
+    <t>ДБТ Созопол</t>
+  </si>
+  <si>
+    <t>ДБТ Варна</t>
+  </si>
+  <si>
+    <t>ДБТ Вълчи Дол</t>
+  </si>
+  <si>
+    <t>ДБТ Генерал Тошево</t>
+  </si>
+  <si>
+    <t>ДБТ Долни Чифлик</t>
+  </si>
+  <si>
+    <t>ДБТ Каварна</t>
+  </si>
+  <si>
+    <t>ДБТ Каолиново</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ДБТ Нови Пазар </t>
+  </si>
+  <si>
+    <t>ДБТ Велики Преслав</t>
+  </si>
+  <si>
+    <t>ДБТ Провадия</t>
+  </si>
+  <si>
+    <t>ДБТ Тервел</t>
+  </si>
+  <si>
+    <t>ДБТ Добрич</t>
+  </si>
+  <si>
+    <t>ДБТ Шумен</t>
+  </si>
+  <si>
+    <t>ДБТ Велико Търново</t>
+  </si>
+  <si>
+    <t>ДБТ Габрово</t>
+  </si>
+  <si>
+    <t>ДБТ Горна Оряховица</t>
+  </si>
+  <si>
+    <t>ДБТ Долна Митрополия</t>
+  </si>
+  <si>
+    <t>ДБТ Левски</t>
+  </si>
+  <si>
+    <t>ДБТ Ловеч</t>
+  </si>
+  <si>
+    <t>ДБТ Луковит</t>
+  </si>
+  <si>
+    <t>ДБТ Никопол</t>
+  </si>
+  <si>
+    <t>ДБТ Павликени</t>
+  </si>
+  <si>
+    <t>ДБТ Плевен</t>
+  </si>
+  <si>
+    <t>ДБТ Свищов</t>
+  </si>
+  <si>
+    <t>ДБТ Тетевен</t>
+  </si>
+  <si>
+    <t>ДБТ Троян</t>
+  </si>
+  <si>
+    <t>ДБТ Червен Бряг</t>
+  </si>
+  <si>
+    <t>ДБТ Белоградчик</t>
+  </si>
+  <si>
+    <t>ДБТ Берковица</t>
+  </si>
+  <si>
+    <t>ДБТ Бяла Слатина</t>
+  </si>
+  <si>
+    <t>ДБТ Видин</t>
+  </si>
+  <si>
+    <t>ДБТ Враца</t>
+  </si>
+  <si>
+    <t>ДБТ Козлодуй</t>
+  </si>
+  <si>
+    <t>ДБТ Кула</t>
+  </si>
+  <si>
+    <t>ДБТ Лом</t>
+  </si>
+  <si>
+    <t>ДБТ Мездра</t>
+  </si>
+  <si>
+    <t>ДБТ Монтана</t>
+  </si>
+  <si>
+    <t>ДБТ Оряхово</t>
+  </si>
+  <si>
+    <t>ДБТ Асеновград</t>
+  </si>
+  <si>
+    <t>ДБТ Велинград</t>
+  </si>
+  <si>
+    <t>ДБТ Девин</t>
+  </si>
+  <si>
+    <t>ДБТ Златоград</t>
+  </si>
+  <si>
+    <t>ДБТ Карлово</t>
+  </si>
+  <si>
+    <t>ДБТ Мадан</t>
+  </si>
+  <si>
+    <t>ДБТ Пловдив-Марица</t>
+  </si>
+  <si>
+    <t>ДБТ Пазарджик</t>
+  </si>
+  <si>
+    <t>ДБТ Панагюрище</t>
+  </si>
+  <si>
+    <t>ДБТ Пещера</t>
+  </si>
+  <si>
+    <t>ДБТ Пловдив</t>
+  </si>
+  <si>
+    <t>ДБТ Първомай</t>
+  </si>
+  <si>
+    <t>ДБТ Пловдив-Родопи</t>
+  </si>
+  <si>
+    <t>ДБТ Септември</t>
+  </si>
+  <si>
+    <t>ДБТ Смолян</t>
+  </si>
+  <si>
+    <t>ДБТ Бяла</t>
+  </si>
+  <si>
+    <t>ДБТ Ветово</t>
+  </si>
+  <si>
+    <t>ДБТ Дулово</t>
+  </si>
+  <si>
+    <t>ДБТ Исперих</t>
+  </si>
+  <si>
+    <t>ДБТ Кубрат</t>
+  </si>
+  <si>
+    <t>ДБТ Омуртаг</t>
+  </si>
+  <si>
+    <t>ДБТ Попово</t>
+  </si>
+  <si>
+    <t>ДБТ Разград</t>
+  </si>
+  <si>
+    <t>ДБТ Тутракан</t>
+  </si>
+  <si>
+    <t>ДБТ Търговище</t>
+  </si>
+  <si>
+    <t>ДБТ Русе</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1023,11 +1330,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="B107" sqref="B107"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B80" sqref="B80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1042,7 +1349,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>212</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1053,7 +1360,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>213</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -1064,7 +1371,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>214</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -1075,7 +1382,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>215</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
@@ -1086,7 +1393,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>243</v>
       </c>
       <c r="C5" t="s">
         <v>29</v>
@@ -1097,7 +1404,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>244</v>
       </c>
       <c r="C6" t="s">
         <v>31</v>
@@ -1108,7 +1415,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>245</v>
       </c>
       <c r="C7" t="s">
         <v>35</v>
@@ -1119,7 +1426,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>246</v>
       </c>
       <c r="C8" t="s">
         <v>37</v>
@@ -1130,7 +1437,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>247</v>
       </c>
       <c r="C9" t="s">
         <v>41</v>
@@ -1141,7 +1448,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>248</v>
       </c>
       <c r="C10" t="s">
         <v>43</v>
@@ -1152,7 +1459,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>46</v>
+        <v>249</v>
       </c>
       <c r="C11" t="s">
         <v>47</v>
@@ -1163,7 +1470,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>48</v>
+        <v>250</v>
       </c>
       <c r="C12" t="s">
         <v>49</v>
@@ -1174,7 +1481,7 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>52</v>
+        <v>251</v>
       </c>
       <c r="C13" t="s">
         <v>53</v>
@@ -1185,7 +1492,7 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>54</v>
+        <v>252</v>
       </c>
       <c r="C14" t="s">
         <v>55</v>
@@ -1196,7 +1503,7 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>58</v>
+        <v>253</v>
       </c>
       <c r="C15" t="s">
         <v>59</v>
@@ -1207,7 +1514,7 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>60</v>
+        <v>254</v>
       </c>
       <c r="C16" t="s">
         <v>61</v>
@@ -1218,7 +1525,7 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>62</v>
+        <v>255</v>
       </c>
       <c r="C17" t="s">
         <v>63</v>
@@ -1229,7 +1536,7 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>66</v>
+        <v>256</v>
       </c>
       <c r="C18" t="s">
         <v>67</v>
@@ -1240,7 +1547,7 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>68</v>
+        <v>257</v>
       </c>
       <c r="C19" t="s">
         <v>69</v>
@@ -1251,7 +1558,7 @@
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>72</v>
+        <v>258</v>
       </c>
       <c r="C20" t="s">
         <v>73</v>
@@ -1262,7 +1569,7 @@
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>74</v>
+        <v>259</v>
       </c>
       <c r="C21" t="s">
         <v>75</v>
@@ -1273,7 +1580,7 @@
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>78</v>
+        <v>260</v>
       </c>
       <c r="C22" t="s">
         <v>79</v>
@@ -1284,7 +1591,7 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>80</v>
+        <v>261</v>
       </c>
       <c r="C23" t="s">
         <v>81</v>
@@ -1295,7 +1602,7 @@
         <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>82</v>
+        <v>262</v>
       </c>
       <c r="C24" t="s">
         <v>83</v>
@@ -1306,7 +1613,7 @@
         <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>84</v>
+        <v>263</v>
       </c>
       <c r="C25" t="s">
         <v>85</v>
@@ -1317,7 +1624,7 @@
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>86</v>
+        <v>264</v>
       </c>
       <c r="C26" t="s">
         <v>87</v>
@@ -1328,7 +1635,7 @@
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>90</v>
+        <v>265</v>
       </c>
       <c r="C27" t="s">
         <v>91</v>
@@ -1339,7 +1646,7 @@
         <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>94</v>
+        <v>266</v>
       </c>
       <c r="C28" t="s">
         <v>95</v>
@@ -1350,7 +1657,7 @@
         <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>96</v>
+        <v>267</v>
       </c>
       <c r="C29" t="s">
         <v>97</v>
@@ -1361,7 +1668,7 @@
         <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>98</v>
+        <v>268</v>
       </c>
       <c r="C30" t="s">
         <v>99</v>
@@ -1372,7 +1679,7 @@
         <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>100</v>
+        <v>269</v>
       </c>
       <c r="C31" t="s">
         <v>101</v>
@@ -1383,7 +1690,7 @@
         <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>104</v>
+        <v>270</v>
       </c>
       <c r="C32" t="s">
         <v>105</v>
@@ -1394,7 +1701,7 @@
         <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>108</v>
+        <v>271</v>
       </c>
       <c r="C33" t="s">
         <v>109</v>
@@ -1405,7 +1712,7 @@
         <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>110</v>
+        <v>272</v>
       </c>
       <c r="C34" t="s">
         <v>111</v>
@@ -1416,7 +1723,7 @@
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>114</v>
+        <v>273</v>
       </c>
       <c r="C35" t="s">
         <v>115</v>
@@ -1427,7 +1734,7 @@
         <v>36</v>
       </c>
       <c r="B36" t="s">
-        <v>116</v>
+        <v>274</v>
       </c>
       <c r="C36" t="s">
         <v>117</v>
@@ -1438,7 +1745,7 @@
         <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>120</v>
+        <v>275</v>
       </c>
       <c r="C37" t="s">
         <v>121</v>
@@ -1449,7 +1756,7 @@
         <v>38</v>
       </c>
       <c r="B38" t="s">
-        <v>122</v>
+        <v>276</v>
       </c>
       <c r="C38" t="s">
         <v>123</v>
@@ -1460,7 +1767,7 @@
         <v>39</v>
       </c>
       <c r="B39" t="s">
-        <v>126</v>
+        <v>277</v>
       </c>
       <c r="C39" t="s">
         <v>127</v>
@@ -1471,7 +1778,7 @@
         <v>40</v>
       </c>
       <c r="B40" t="s">
-        <v>128</v>
+        <v>278</v>
       </c>
       <c r="C40" t="s">
         <v>129</v>
@@ -1482,7 +1789,7 @@
         <v>41</v>
       </c>
       <c r="B41" t="s">
-        <v>130</v>
+        <v>279</v>
       </c>
       <c r="C41" t="s">
         <v>131</v>
@@ -1493,7 +1800,7 @@
         <v>42</v>
       </c>
       <c r="B42" t="s">
-        <v>132</v>
+        <v>280</v>
       </c>
       <c r="C42" t="s">
         <v>133</v>
@@ -1504,7 +1811,7 @@
         <v>43</v>
       </c>
       <c r="B43" t="s">
-        <v>152</v>
+        <v>281</v>
       </c>
       <c r="C43" t="s">
         <v>153</v>
@@ -1515,7 +1822,7 @@
         <v>44</v>
       </c>
       <c r="B44" t="s">
-        <v>156</v>
+        <v>282</v>
       </c>
       <c r="C44" t="s">
         <v>157</v>
@@ -1526,7 +1833,7 @@
         <v>45</v>
       </c>
       <c r="B45" t="s">
-        <v>158</v>
+        <v>283</v>
       </c>
       <c r="C45" t="s">
         <v>159</v>
@@ -1537,7 +1844,7 @@
         <v>46</v>
       </c>
       <c r="B46" t="s">
-        <v>160</v>
+        <v>284</v>
       </c>
       <c r="C46" t="s">
         <v>161</v>
@@ -1548,7 +1855,7 @@
         <v>47</v>
       </c>
       <c r="B47" t="s">
-        <v>164</v>
+        <v>285</v>
       </c>
       <c r="C47" t="s">
         <v>165</v>
@@ -1559,7 +1866,7 @@
         <v>48</v>
       </c>
       <c r="B48" t="s">
-        <v>166</v>
+        <v>286</v>
       </c>
       <c r="C48" t="s">
         <v>167</v>
@@ -1570,7 +1877,7 @@
         <v>49</v>
       </c>
       <c r="B49" t="s">
-        <v>170</v>
+        <v>287</v>
       </c>
       <c r="C49" t="s">
         <v>171</v>
@@ -1581,7 +1888,7 @@
         <v>50</v>
       </c>
       <c r="B50" t="s">
-        <v>172</v>
+        <v>288</v>
       </c>
       <c r="C50" t="s">
         <v>173</v>
@@ -1592,7 +1899,7 @@
         <v>51</v>
       </c>
       <c r="B51" t="s">
-        <v>176</v>
+        <v>289</v>
       </c>
       <c r="C51" t="s">
         <v>177</v>
@@ -1603,7 +1910,7 @@
         <v>52</v>
       </c>
       <c r="B52" t="s">
-        <v>178</v>
+        <v>290</v>
       </c>
       <c r="C52" t="s">
         <v>179</v>
@@ -1614,7 +1921,7 @@
         <v>53</v>
       </c>
       <c r="B53" t="s">
-        <v>180</v>
+        <v>291</v>
       </c>
       <c r="C53" t="s">
         <v>181</v>
@@ -1625,7 +1932,7 @@
         <v>54</v>
       </c>
       <c r="B54" t="s">
-        <v>184</v>
+        <v>292</v>
       </c>
       <c r="C54" t="s">
         <v>185</v>
@@ -1636,7 +1943,7 @@
         <v>55</v>
       </c>
       <c r="B55" t="s">
-        <v>188</v>
+        <v>293</v>
       </c>
       <c r="C55" t="s">
         <v>189</v>
@@ -1647,7 +1954,7 @@
         <v>56</v>
       </c>
       <c r="B56" t="s">
-        <v>192</v>
+        <v>294</v>
       </c>
       <c r="C56" t="s">
         <v>193</v>
@@ -1658,7 +1965,7 @@
         <v>57</v>
       </c>
       <c r="B57" t="s">
-        <v>194</v>
+        <v>295</v>
       </c>
       <c r="C57" t="s">
         <v>195</v>
@@ -1669,7 +1976,7 @@
         <v>58</v>
       </c>
       <c r="B58" t="s">
-        <v>196</v>
+        <v>296</v>
       </c>
       <c r="C58" t="s">
         <v>197</v>
@@ -1680,7 +1987,7 @@
         <v>59</v>
       </c>
       <c r="B59" t="s">
-        <v>198</v>
+        <v>297</v>
       </c>
       <c r="C59" t="s">
         <v>199</v>
@@ -1691,7 +1998,7 @@
         <v>60</v>
       </c>
       <c r="B60" t="s">
-        <v>200</v>
+        <v>298</v>
       </c>
       <c r="C60" t="s">
         <v>201</v>
@@ -1702,7 +2009,7 @@
         <v>61</v>
       </c>
       <c r="B61" t="s">
-        <v>206</v>
+        <v>299</v>
       </c>
       <c r="C61" t="s">
         <v>207</v>
@@ -1713,7 +2020,7 @@
         <v>62</v>
       </c>
       <c r="B62" t="s">
-        <v>208</v>
+        <v>300</v>
       </c>
       <c r="C62" t="s">
         <v>209</v>
@@ -1724,7 +2031,7 @@
         <v>63</v>
       </c>
       <c r="B63" t="s">
-        <v>204</v>
+        <v>301</v>
       </c>
       <c r="C63" t="s">
         <v>205</v>
@@ -1735,7 +2042,7 @@
         <v>64</v>
       </c>
       <c r="B64" t="s">
-        <v>202</v>
+        <v>302</v>
       </c>
       <c r="C64" t="s">
         <v>203</v>
@@ -1746,7 +2053,7 @@
         <v>65</v>
       </c>
       <c r="B65" t="s">
-        <v>190</v>
+        <v>303</v>
       </c>
       <c r="C65" t="s">
         <v>191</v>
@@ -1757,7 +2064,7 @@
         <v>66</v>
       </c>
       <c r="B66" t="s">
-        <v>186</v>
+        <v>304</v>
       </c>
       <c r="C66" t="s">
         <v>187</v>
@@ -1768,7 +2075,7 @@
         <v>67</v>
       </c>
       <c r="B67" t="s">
-        <v>182</v>
+        <v>305</v>
       </c>
       <c r="C67" t="s">
         <v>183</v>
@@ -1779,7 +2086,7 @@
         <v>68</v>
       </c>
       <c r="B68" t="s">
-        <v>174</v>
+        <v>306</v>
       </c>
       <c r="C68" t="s">
         <v>175</v>
@@ -1790,7 +2097,7 @@
         <v>69</v>
       </c>
       <c r="B69" t="s">
-        <v>168</v>
+        <v>307</v>
       </c>
       <c r="C69" t="s">
         <v>169</v>
@@ -1801,7 +2108,7 @@
         <v>70</v>
       </c>
       <c r="B70" t="s">
-        <v>162</v>
+        <v>308</v>
       </c>
       <c r="C70" t="s">
         <v>163</v>
@@ -1812,7 +2119,7 @@
         <v>71</v>
       </c>
       <c r="B71" t="s">
-        <v>154</v>
+        <v>309</v>
       </c>
       <c r="C71" t="s">
         <v>155</v>
@@ -1823,7 +2130,7 @@
         <v>72</v>
       </c>
       <c r="B72" t="s">
-        <v>150</v>
+        <v>310</v>
       </c>
       <c r="C72" t="s">
         <v>151</v>
@@ -1834,7 +2141,7 @@
         <v>73</v>
       </c>
       <c r="B73" t="s">
-        <v>148</v>
+        <v>311</v>
       </c>
       <c r="C73" t="s">
         <v>149</v>
@@ -1845,7 +2152,7 @@
         <v>74</v>
       </c>
       <c r="B74" t="s">
-        <v>146</v>
+        <v>312</v>
       </c>
       <c r="C74" t="s">
         <v>147</v>
@@ -1856,7 +2163,7 @@
         <v>75</v>
       </c>
       <c r="B75" t="s">
-        <v>144</v>
+        <v>313</v>
       </c>
       <c r="C75" t="s">
         <v>145</v>
@@ -1867,7 +2174,7 @@
         <v>76</v>
       </c>
       <c r="B76" t="s">
-        <v>140</v>
+        <v>227</v>
       </c>
       <c r="C76" t="s">
         <v>141</v>
@@ -1878,7 +2185,7 @@
         <v>77</v>
       </c>
       <c r="B77" t="s">
-        <v>138</v>
+        <v>314</v>
       </c>
       <c r="C77" t="s">
         <v>139</v>
@@ -1889,7 +2196,7 @@
         <v>78</v>
       </c>
       <c r="B78" t="s">
-        <v>136</v>
+        <v>315</v>
       </c>
       <c r="C78" t="s">
         <v>137</v>
@@ -1900,7 +2207,7 @@
         <v>79</v>
       </c>
       <c r="B79" t="s">
-        <v>134</v>
+        <v>316</v>
       </c>
       <c r="C79" t="s">
         <v>135</v>
@@ -1911,7 +2218,7 @@
         <v>80</v>
       </c>
       <c r="B80" t="s">
-        <v>124</v>
+        <v>216</v>
       </c>
       <c r="C80" t="s">
         <v>125</v>
@@ -1922,7 +2229,7 @@
         <v>81</v>
       </c>
       <c r="B81" t="s">
-        <v>10</v>
+        <v>217</v>
       </c>
       <c r="C81" t="s">
         <v>11</v>
@@ -1933,7 +2240,7 @@
         <v>82</v>
       </c>
       <c r="B82" t="s">
-        <v>118</v>
+        <v>218</v>
       </c>
       <c r="C82" t="s">
         <v>119</v>
@@ -1944,7 +2251,7 @@
         <v>83</v>
       </c>
       <c r="B83" t="s">
-        <v>12</v>
+        <v>219</v>
       </c>
       <c r="C83" t="s">
         <v>13</v>
@@ -1955,7 +2262,7 @@
         <v>84</v>
       </c>
       <c r="B84" t="s">
-        <v>112</v>
+        <v>220</v>
       </c>
       <c r="C84" t="s">
         <v>113</v>
@@ -1966,7 +2273,7 @@
         <v>85</v>
       </c>
       <c r="B85" t="s">
-        <v>14</v>
+        <v>221</v>
       </c>
       <c r="C85" t="s">
         <v>15</v>
@@ -1977,7 +2284,7 @@
         <v>86</v>
       </c>
       <c r="B86" t="s">
-        <v>106</v>
+        <v>222</v>
       </c>
       <c r="C86" t="s">
         <v>107</v>
@@ -1988,7 +2295,7 @@
         <v>87</v>
       </c>
       <c r="B87" t="s">
-        <v>102</v>
+        <v>223</v>
       </c>
       <c r="C87" t="s">
         <v>103</v>
@@ -1999,7 +2306,7 @@
         <v>88</v>
       </c>
       <c r="B88" t="s">
-        <v>16</v>
+        <v>224</v>
       </c>
       <c r="C88" t="s">
         <v>17</v>
@@ -2010,7 +2317,7 @@
         <v>89</v>
       </c>
       <c r="B89" t="s">
-        <v>210</v>
+        <v>225</v>
       </c>
       <c r="C89" t="s">
         <v>211</v>
@@ -2021,7 +2328,7 @@
         <v>90</v>
       </c>
       <c r="B90" t="s">
-        <v>20</v>
+        <v>226</v>
       </c>
       <c r="C90" t="s">
         <v>21</v>
@@ -2032,7 +2339,7 @@
         <v>91</v>
       </c>
       <c r="B91" t="s">
-        <v>22</v>
+        <v>227</v>
       </c>
       <c r="C91" t="s">
         <v>23</v>
@@ -2043,7 +2350,7 @@
         <v>92</v>
       </c>
       <c r="B92" t="s">
-        <v>26</v>
+        <v>228</v>
       </c>
       <c r="C92" t="s">
         <v>27</v>
@@ -2054,7 +2361,7 @@
         <v>93</v>
       </c>
       <c r="B93" t="s">
-        <v>92</v>
+        <v>229</v>
       </c>
       <c r="C93" t="s">
         <v>93</v>
@@ -2065,7 +2372,7 @@
         <v>94</v>
       </c>
       <c r="B94" t="s">
-        <v>88</v>
+        <v>230</v>
       </c>
       <c r="C94" t="s">
         <v>89</v>
@@ -2076,7 +2383,7 @@
         <v>95</v>
       </c>
       <c r="B95" t="s">
-        <v>76</v>
+        <v>231</v>
       </c>
       <c r="C95" t="s">
         <v>77</v>
@@ -2087,7 +2394,7 @@
         <v>96</v>
       </c>
       <c r="B96" t="s">
-        <v>70</v>
+        <v>232</v>
       </c>
       <c r="C96" t="s">
         <v>71</v>
@@ -2098,7 +2405,7 @@
         <v>97</v>
       </c>
       <c r="B97" t="s">
-        <v>64</v>
+        <v>233</v>
       </c>
       <c r="C97" t="s">
         <v>65</v>
@@ -2109,7 +2416,7 @@
         <v>98</v>
       </c>
       <c r="B98" t="s">
-        <v>56</v>
+        <v>234</v>
       </c>
       <c r="C98" t="s">
         <v>57</v>
@@ -2120,7 +2427,7 @@
         <v>99</v>
       </c>
       <c r="B99" t="s">
-        <v>50</v>
+        <v>235</v>
       </c>
       <c r="C99" t="s">
         <v>51</v>
@@ -2131,7 +2438,7 @@
         <v>100</v>
       </c>
       <c r="B100" t="s">
-        <v>44</v>
+        <v>236</v>
       </c>
       <c r="C100" t="s">
         <v>45</v>
@@ -2142,7 +2449,7 @@
         <v>101</v>
       </c>
       <c r="B101" t="s">
-        <v>38</v>
+        <v>237</v>
       </c>
       <c r="C101" t="s">
         <v>39</v>
@@ -2153,7 +2460,7 @@
         <v>102</v>
       </c>
       <c r="B102" t="s">
-        <v>32</v>
+        <v>238</v>
       </c>
       <c r="C102" t="s">
         <v>33</v>
@@ -2164,7 +2471,7 @@
         <v>103</v>
       </c>
       <c r="B103" t="s">
-        <v>24</v>
+        <v>239</v>
       </c>
       <c r="C103" t="s">
         <v>25</v>
@@ -2175,7 +2482,7 @@
         <v>104</v>
       </c>
       <c r="B104" t="s">
-        <v>18</v>
+        <v>240</v>
       </c>
       <c r="C104" t="s">
         <v>19</v>
@@ -2186,7 +2493,7 @@
         <v>105</v>
       </c>
       <c r="B105" t="s">
-        <v>142</v>
+        <v>241</v>
       </c>
       <c r="C105" t="s">
         <v>143</v>
@@ -2197,14 +2504,14 @@
         <v>106</v>
       </c>
       <c r="B106" t="s">
-        <v>8</v>
+        <v>242</v>
       </c>
       <c r="C106" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="B1:C107">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B1:C107">
     <sortCondition ref="C1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2213,7 +2520,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C106"/>
   <sheetViews>
     <sheetView topLeftCell="A82" workbookViewId="0">

</xml_diff>